<commit_message>
readd my version of F0AM to get versions aligned
</commit_message>
<xml_diff>
--- a/F0AM-4.3.0.1/Chem/Photolysis/PhotoDataSources_updated_072025.xlsx
+++ b/F0AM-4.3.0.1/Chem/Photolysis/PhotoDataSources_updated_072025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessasun/Documents/phd/utah/research/USOS_shared/F0AM-4.3.0.1/Chem/Photolysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1030AA5-ACD6-AD4A-B075-159638A68B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43968AC9-D320-7A4C-A79F-EB0F5E91CD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15020" yWindow="740" windowWidth="29900" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38760" yWindow="4420" windowWidth="29900" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2026,6 +2026,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2055,10 +2059,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2410,8 +2410,8 @@
   <dimension ref="A1:T1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -2439,33 +2439,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="I1" s="66" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="I1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
-      <c r="M1" s="69" t="s">
+      <c r="J1" s="69"/>
+      <c r="K1" s="70"/>
+      <c r="M1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="70"/>
-      <c r="O1" s="71"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="73"/>
       <c r="Q1" s="9" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="65"/>
+      <c r="A2" s="67"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -4171,10 +4171,10 @@
       <c r="E46" s="3"/>
       <c r="F46" s="25"/>
       <c r="H46" s="26"/>
-      <c r="I46" s="73"/>
+      <c r="I46" s="63"/>
       <c r="J46" s="29"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="72"/>
+      <c r="L46" s="62"/>
       <c r="M46" s="32"/>
       <c r="N46" s="20"/>
       <c r="O46" s="1"/>

</xml_diff>